<commit_message>
Refactor stemming function and improve moral classification logic, and add code to scrape proverbs from websites and classify them based on morals
</commit_message>
<xml_diff>
--- a/manners.xlsx
+++ b/manners.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/942a79fd4481367f/Desktop/WebScraping/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_050D2855D020F5347A600854B5A82487797899FE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFCDE509-2585-404B-A6D0-3F32336C0641}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="manners" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="456">
   <si>
     <t>Citation</t>
   </si>
@@ -707,13 +701,696 @@
   </si>
   <si>
     <t xml:space="preserve"> ومن لا يتق الشَّتْمَ يُشْتَم.</t>
+  </si>
+  <si>
+    <t>الصبر شجرة جذورها مُرّة وثمرها لذيذ.</t>
+  </si>
+  <si>
+    <t>Good Moral: صَبْر</t>
+  </si>
+  <si>
+    <t>الصبر هو أفضل شيء يمكنك استخدامه مع مرور الوقت إذا أصابك الأذى.</t>
+  </si>
+  <si>
+    <t>ثق بصبرك وكن حذرا في الليالي، لأنها بلدان.</t>
+  </si>
+  <si>
+    <t>النجاح والغنى يتبعان الصبر، وستر الفقر نسيج الكسل.</t>
+  </si>
+  <si>
+    <t>وبحسب الطفل، إذا لم يحصل على ما يريد بالصبر، فإنه يبقى فوق الصبر.</t>
+  </si>
+  <si>
+    <t>الغرور نصف الداء، والطمأنينة نصف العلاج، والصبر أول خطوة للشفاء.</t>
+  </si>
+  <si>
+    <t>عندما يشتد الألم ويزداد الألم، لا يوجد علاج فوري وفعال مثل وصفة الصبر والصلاة لتهدئة النفس وعودتها إلى طبيعتها.</t>
+  </si>
+  <si>
+    <t>واعلم أن أعلى درجات الصداقة اثنتين أن تصبر على صديقك عندما تسود طبعه فيسيء إليك، ثم عندما تسود طبيعتك تصبر حتى لا تسيء إليه.</t>
+  </si>
+  <si>
+    <t>فالصبر مطلوب حتى يخرج العباد من المشاكل.</t>
+  </si>
+  <si>
+    <t>عليك أن تنتظر حتى المساء لتعرف كم كان يومك رائعًا.</t>
+  </si>
+  <si>
+    <t>قليل من الصبر يساوي عشر سنوات من الراحة.</t>
+  </si>
+  <si>
+    <t>إلا بالصبر تنال مرادك، وبالتقوى يلين لك الحديد.</t>
+  </si>
+  <si>
+    <t>اصبر قليلاً، فإن بعد العسر يسراً، ولكل أمر وقته واتجاهه، وفي أحوالنا لمحة من الحقيقة، وهناك تقدير فوق تقديرنا لله.</t>
+  </si>
+  <si>
+    <t>فحسن الصبر ليس فيه شكوى، وحسن العفو ليس فيه ضرر، وحسن الهجر ليس فيه إدانة.</t>
+  </si>
+  <si>
+    <t>علمني الزمن، وعلمني الصبر، وأقنعني الرزق، وكفاني اليأس، وتعرضت للفتنة حتى حرمت من نهاني.</t>
+  </si>
+  <si>
+    <t>الصبر هو أفضل شيء يمكنك استخدامه ضد الزمن إذا أصابك أي ضرر.</t>
+  </si>
+  <si>
+    <t>استعين بالله عز وجل، والجأ إليه واطلب منه أن يلهمك الصبر على حكمه حتى يخفف البلاء وتنجح في الاختبار.</t>
+  </si>
+  <si>
+    <t>الصبر سلعة تدفع فيها المال ثم يضاعفه لك ثم تؤجله.</t>
+  </si>
+  <si>
+    <t>ولكي يتحقق الصبر لا بد من طلب المساعدة والثقة.</t>
+  </si>
+  <si>
+    <t>الصبر على الألم يأتي في الصدمة الأولى.</t>
+  </si>
+  <si>
+    <t>احفظ لسانك من كثرة الشكوى في بعض الأحيان، واصبر على المشاكل وارضى بما قسمه الله لك، فإنك لا تدري ما مصيرك.</t>
+  </si>
+  <si>
+    <t>فالغضب لا يتوافق مع الصبر، والشكوى لا تتوافق مع الرضا، فهما ضد بعضهما البعض.</t>
+  </si>
+  <si>
+    <t>الطمأنينة أول خطوة في العلاج، والخطأ نصف الداء، والصبر أول طريق الشفاء.</t>
+  </si>
+  <si>
+    <t>الصيد والعيش في الصحراء يعلم الصبر، لأنه عليك الانتظار حتى تحصل على الجميلات والطعام، لذلك علم نفسك وأولادك الصيد والانتظار حتى تحصل على ما تريد.</t>
+  </si>
+  <si>
+    <t>الصبر والمرونة هي الصفات التي نحب أن ننميها في أطفالنا لمساعدتهم على البقاء في الحياة، وهما من أهم الصفات التي ستساعدهم على تحقيق أحلامهم دون استسلام.</t>
+  </si>
+  <si>
+    <t>وتذكر حال من هو أكثر اضطراباً منك؛  لأن من رأى متاعب غيره تهون عليه متاعبه.</t>
+  </si>
+  <si>
+    <t>الصبر على مواجهة المتاعب، والاستهانة بأثر الشوك تحت الأقدام.</t>
+  </si>
+  <si>
+    <t>يا ابن آدم، لماذا تحزن على خسارة لا يردها لك الموت، وكيف تفرح على هدية لم يتركها الموت بين يديك؟</t>
+  </si>
+  <si>
+    <t>بالنسبة لي فإن قضمة الجمرة أو الإمساك بها بيدي حتى تبرد أحب من قول “ليت الأمر لم يكن هكذا، اصبر على البلاء” إلى أمر قد كتبه الله.</t>
+  </si>
+  <si>
+    <t>فالمصيبة قدر الله لا مفر منه، ولا يأتي قدر الله إلا بالخير.</t>
+  </si>
+  <si>
+    <t>إن الرضا بقضاء الله وقدره والتعرض للمصائب من أعظم ما يعين العبد على مواجهة البلاء.</t>
+  </si>
+  <si>
+    <t>ولا ينفع القلق والسخط، لأن الندم على ما فاته لا يحدثه.</t>
+  </si>
+  <si>
+    <t>أن تعلم طبيعة الدنيا وأنها دار عناء، كما أن الدنيا جسر يوصلك إلى دار الآخرة، فلا تقلق من الأشياء التي تفوتك في الدنيا واصبر.</t>
+  </si>
+  <si>
+    <t>ثق أنه سيكون هناك فرج من الله عز وجل، اصبر وانتظر الخلاص عندما ترى شيئًا لا يمكنك فعله بطريقة أخرى.</t>
+  </si>
+  <si>
+    <t>استعيني بالله، ولجأي إليه، واستعيني به، واسأليه أن يلهمك الصبر والرضا بقضاءه.  لتسهيل تجربة الملل والنجاح في الامتحان.</t>
+  </si>
+  <si>
+    <t>للحصول على الصبر، من الضروري الثقة وطلب المساعدة.</t>
+  </si>
+  <si>
+    <t>إن الثقة بالله أمر كبير كثيرا ما نتجاهله، ونحن اليوم بحاجة إلى هذه الثقة لاستعادة توازن الحياة المضطرب.</t>
+  </si>
+  <si>
+    <t>توكل على الله تجد إبراهيم حين ألقي في النار فقال بعزة المتوكلين حسبنا الله ونعم الوكيل، فجاء الأمر الإلهي يا نار وتكون بردا وسلاما على إبراهيم.</t>
+  </si>
+  <si>
+    <t>توكلت هاجر على الله عندما يموت زوجها ويتركها في وادٍ غير مثمر، في صحراء قاحلة، في شمس حارقة موحشة، وتقول يا إبراهيم، لمن تتركنا؟  واستمرت جهوده إلى الأبد.  ولو كنا خائفين وجزعين لما حصلنا اليوم على بركات ماء زمزم.</t>
+  </si>
+  <si>
+    <t>توكل على الله في الذين قيل أن الناس قد جمعوا عليك.  الخوف منهم؛  ولكن ثقتهم بالله أكبر من قوة أعدائهم وعددهم.</t>
+  </si>
+  <si>
+    <t>الثقة بالله هي السعادة في الحياة، الثقة بالنفس، قرة العين، أغنية السعداء.</t>
+  </si>
+  <si>
+    <t>التوكل على الله لا يخيف الإنسان، فهي قاعدة الصبر والتفاؤل.</t>
+  </si>
+  <si>
+    <t>الثقة بالله لا تجعل الإنسان حزيناً أو مهموماً.</t>
+  </si>
+  <si>
+    <t>الثقة بالله هي أول خطوة للنجاح وأساس الصبر والتفاؤل.</t>
+  </si>
+  <si>
+    <t>والإيمان بالله مرتبط بالصبر، لأن الصابر هو الذي يؤمن أن الله سيحسن إليه.</t>
+  </si>
+  <si>
+    <t>الحب في الحقيقة هو أجمل وأحلى أنواع الصبر.</t>
+  </si>
+  <si>
+    <t>ومن لا يعرف الصبر لا يعرف الحب.</t>
+  </si>
+  <si>
+    <t>أهم شيء في الحياة الزوجية هو الصبر وليس الحب، فالحب لا يمكن أن يستمر طويلاً.</t>
+  </si>
+  <si>
+    <t>الحب هو أجمل اكتشاف للإنسان، وإلا لكان مجرد صخرة لا يحركها شيء، ولا شيء سوى تآكل يومي، والحب أيضًا يتآكل عندما يفتقر إلى الإبداع المستمر.</t>
+  </si>
+  <si>
+    <t>لا تؤذي شخصاً ثم تقول أحبك، لا تحزنه ثم تقول ما يؤذيني سيؤذيك أيضاً، لا تزرع الشوك في صدره ثم تقول أهتم بك، الحب الحقيقي لا يؤذيك. لا تظهر جوهرها غير العاطفة.  ، الغضب والغياب والخلاف، ولكن في المواقف العادية الهدوء والرومانسية، من السهل التظاهر والسيطرة، أحب السادة الصبر، نعم الصبر.</t>
+  </si>
+  <si>
+    <t>وأنا هنا أتحدث عن الحب الإنساني بمعناه الواسع والجميل والواسع، في العلاقة بين الرجل والمرأة، سواء كانت حلالاً أو حراماً، صحاً أو خطأً، وليس اختزالاً في واقعنا الحالي، فالحب هو الصبر.</t>
+  </si>
+  <si>
+    <t>عندما أحب الصحابة الله ورسوله وقدموا هذا الحب على أنفسهم وأموالهم وأولادهم، ضحوا بكل شيء وتحملوا العذاب والجوع والتشريد والموت، فأي حب وأي صبر؟</t>
+  </si>
+  <si>
+    <t>ألم تر كيف تصبر الأمهات على الحمل والألم والثقل والتعب حتى قبل رؤية مولودهن الجديد، ثم يختبرن عذاب الولادة، لكن عندما يحتضن الصغير عينيه فقط ينسى كل الألم، بل على العكس فهو يعاني أكثر.  يعذبها فقط لأنها تحبه.</t>
+  </si>
+  <si>
+    <t>لقد أدرك فجأة ما كان يتمناه.</t>
+  </si>
+  <si>
+    <t>وهو أيضاً صبر ظفر.</t>
+  </si>
+  <si>
+    <t>لا أصبر على نفسي ولا يصبر الناس علي.</t>
+  </si>
+  <si>
+    <t>دواء الدهر هو الصبر .</t>
+  </si>
+  <si>
+    <t>أجمل أخلاق الناس الصبر.</t>
+  </si>
+  <si>
+    <t>لأن نتيجة الصبر الجميل جميلة.</t>
+  </si>
+  <si>
+    <t>الرضا دليل الثقة، والثقة دليل الشكر، والشكر دليل التكاثر، والزيادة دليل استمرار النعمة، والحياة دليل كل أنواع الخير.</t>
+  </si>
+  <si>
+    <t>يمشي ببطء ويأتي أولاً.</t>
+  </si>
+  <si>
+    <t>الصبر عند الكوارث يسمى إيمانا.</t>
+  </si>
+  <si>
+    <t>الصبر الذي يظهر مع حفظ الأسرار يسمى السرية.</t>
+  </si>
+  <si>
+    <t>إذا كان الصبر مرًا فالنتيجة حلوة.</t>
+  </si>
+  <si>
+    <t>الشخص قليل الصبر مثل المصباح بدون زيت.</t>
+  </si>
+  <si>
+    <t>وكذلك الصبر شجرة جذورها مرة وثمرها لذيذ.</t>
+  </si>
+  <si>
+    <t>وحلاوة الظفر تخفف ألم الصبر.</t>
+  </si>
+  <si>
+    <t>ليس الأمر أن تكون أعمى، بل هو عدم القدرة على تحمل العمى.</t>
+  </si>
+  <si>
+    <t>ومن الجيد أيضًا الصبر على ما يحدث، فإذا صبروا، أحيانًا يكون الصبر مفيدًا.</t>
+  </si>
+  <si>
+    <t>الصبر هو أفضل شيء يمكنك استخدامه مع مرور الوقت إذا كان مضرًا.</t>
+  </si>
+  <si>
+    <t>الله ينتظر لكنه لا يهمل.</t>
+  </si>
+  <si>
+    <t>تماما كما هو الحال اليوم غدا، في مسعدة.</t>
+  </si>
+  <si>
+    <t>أنا أغرق، فما خوفي من البلل؟</t>
+  </si>
+  <si>
+    <t>الشدة والتكلفة.</t>
+  </si>
+  <si>
+    <t>فصبرك على محرمات الله أهون من صبرك على عذاب الله.</t>
+  </si>
+  <si>
+    <t>وكما أن نتيجة الصبر هي النجاح والغنى، كذلك فإن ثوب الفقر هو نتيجة الكسل.</t>
+  </si>
+  <si>
+    <t>تدريجيا تصبح على بينة من الفرص.</t>
+  </si>
+  <si>
+    <t>دع الأيام تفعل ما تشاء واشف نفسك حسب قرار القضاء.</t>
+  </si>
+  <si>
+    <t>إذا كنت تظن أن الصبر عند بعض الناس يساوي البلادة، فلا تخلط بين بلادة الطبيعة المريضة وخضوع الأقوياء لما يصيبهم.</t>
+  </si>
+  <si>
+    <t>فكما زرعت آلامي في حقل الجليد، نلت أيضًا أفراحًا.</t>
+  </si>
+  <si>
+    <t>الصبر هو أفضل دواء للحزن.</t>
+  </si>
+  <si>
+    <t>الوهم نصف الداء، والاطمئنان نصف العلاج، والصبر أول خطوة للشفاء.</t>
+  </si>
+  <si>
+    <t>أحلك ساعات اليوم هي قبل شروق الشمس.</t>
+  </si>
+  <si>
+    <t>كما يسمى الولاء والصبر في سبيل الصداقة.</t>
+  </si>
+  <si>
+    <t>اصبر قليلاً، فإن بعد العسر يسراً، ولكل عمل وقته وإدارته.</t>
+  </si>
+  <si>
+    <t>اصبر على كل مصيبة وضيق واعلم أن الخلود خالد ومرض العيون أهون من العمى.</t>
+  </si>
+  <si>
+    <t>كل قادم قريب وكل قلق على وشك الزوال.</t>
+  </si>
+  <si>
+    <t>ومن لا يصبر على كلمة يسمعها.</t>
+  </si>
+  <si>
+    <t>كما أن الصبر يسمى قوة وإيمانًا عند تحمل الألم.</t>
+  </si>
+  <si>
+    <t>إذا لم تشرب من القذارة مرارا وتكرارا سوف تعطش، فمن الذي سينظف مشروباتك؟</t>
+  </si>
+  <si>
+    <t>اصبر فإن بعد العسر يسرا، ولكل عمل وقته وتدبيره.</t>
+  </si>
+  <si>
+    <t>في الوقت الحاضر.</t>
+  </si>
+  <si>
+    <t>إن التباطؤ من الرحمن، والعجلة من الشيطان.</t>
+  </si>
+  <si>
+    <t>كما أصبر على كل بلاء ومتاعب وأعلم أن الخلود ليس أبدى.</t>
+  </si>
+  <si>
+    <t>هناك أمل عندما تكون السماء مخفية.</t>
+  </si>
+  <si>
+    <t>وقال عمر بن الخطاب (رضي الله عنه) وجدنا خير أرزاقنا، إن خير أرزاقنا ما كسبنا بالصبر، والكرم ولو كان الصبر بين الناس.</t>
+  </si>
+  <si>
+    <t>وكما قال الحسن البصري “الصبر كنز من كنوز الخير لا يعطيه الله إلا عبده الذي يكرمه”.</t>
+  </si>
+  <si>
+    <t>وقال علي بن أبي طالب “لكن الصبر من الإيمان مثل الرأس من الجسد، إذا قطع الرأس صلح الجسد، ثم رفع صوته”.</t>
+  </si>
+  <si>
+    <t>فقال “لا إيمان لمن لا صبر له”.  “الصبر جبل، لا تستسلم، لا تستسلم.”  أمر.</t>
+  </si>
+  <si>
+    <t>وكما قال عبد الله بن مسعود “الإيمان نصفان نصف صبر، ونصف شكر”.</t>
+  </si>
+  <si>
+    <t>وقال أبو علي الدقاق “إن الذين صبروا نالوا عزة الدارين بما نالوا من الله العون”.</t>
+  </si>
+  <si>
+    <t>وكما قال عمر بن عبد العزيز “ما أعطى الله عبداً نعمة فانتزعها منه وعوضها له صابراً، إلا كان ما دفعه خيراً مما حصل”.</t>
+  </si>
+  <si>
+    <t>قال لقمان الحاكم لا شك أن الكلام أقوى من الحجر، وأوثق من الإبرة، وأشد من الصبر، وأدفأ من الجمر.
+    إن في القلوب حقولا، فازرع فيها الكلمة الطيبة، فإنها وإن لم تكن كلها تزدهر، فإن بعضها يزدهر.</t>
+  </si>
+  <si>
+    <t>إن في القلوب حقولا، فازرع فيها الكلمة الطيبة، فإنها وإن لم تكن كلها تزدهر، فإن بعضها يزدهر.</t>
+  </si>
+  <si>
+    <t>وقال علي بن أبي طالب (رضي الله عنه) “الصبر سفر فلا تستسلم”.</t>
+  </si>
+  <si>
+    <t>وكما قال أبو محمد الجريري “ليس الصبر هو التمييز بين النعم والمتاعب، وهدوء البال في كليهما”.</t>
+  </si>
+  <si>
+    <t>قال الحسن الصبر كنز من كنوز الجنة لا يعطيه الله إلا عباده الذين يكرمونه.</t>
+  </si>
+  <si>
+    <t>إذا واجهتك صعوبة يوما ما فلا تجزع، فقد جعل لك اليسر طويلا، ولا تظن بربك سوء الظن، فالله أحق بالنعمة.
+    لو كانت العقول أرزاقاً لكانت الأموال في صف ذوي العقول.</t>
+  </si>
+  <si>
+    <t>لو كانت العقول أرزاقاً لكانت الأموال في صف ذوي العقول.</t>
+  </si>
+  <si>
+    <t>التحلي بالصبر وسوف تنجح.</t>
+  </si>
+  <si>
+    <t>من يرزق فإن رزقه يكفيه، ومن يرزق يكفيه يصبر على الشدائد.</t>
+  </si>
+  <si>
+    <t>أما والله فإما أن تصبر أو تهلك.</t>
+  </si>
+  <si>
+    <t>إذا تعثرت وسقطت في حفرة واسعة فلا تيأس، ستخرج منها أقوى.</t>
+  </si>
+  <si>
+    <t>إن الله مع الصابرين.</t>
+  </si>
+  <si>
+    <t>الصبر هو مفتاح الفرج.</t>
+  </si>
+  <si>
+    <t>عش شهر رجب وسترى العجائب.</t>
+  </si>
+  <si>
+    <t>Good Moral: سِتْر</t>
+  </si>
+  <si>
+    <t>التسامح يهدم الجبال.</t>
+  </si>
+  <si>
+    <t>إن القلق من الكارثة هو كارثة.</t>
+  </si>
+  <si>
+    <t>فإذا تواضع الإنسان شكر إذا أعطي، وإذا رد صبر صبر.</t>
+  </si>
+  <si>
+    <t>Good Moral: شُكْر</t>
+  </si>
+  <si>
+    <t>اصبر على العنب الحامض الذي تأكله.</t>
+  </si>
+  <si>
+    <t>بالصبر تنال ما تريد، وبالتقوى يلين لك الحديد.</t>
+  </si>
+  <si>
+    <t>علمتني اللانهاية، وهداني الصبر، ورزقني الرزق، وأغناني اليأس.</t>
+  </si>
+  <si>
+    <t>اصبر إذا غضبت، اصبر إذا أصابتك مصيبة؛  لأن الليالي حوامل تلد كل معجزة.</t>
+  </si>
+  <si>
+    <t>فالمريض الصابر قد يدرك بعض حاجاته، والمريض المتسرع قد يخطئ.</t>
+  </si>
+  <si>
+    <t>إذا جاءك الزمان بمصيبة فاصبر عليها واشرح لها صدرك؛  لأن مرور الزمن غريب؛  يوماً ما سوف ترى اليسر، ويوماً سوف ترى الصعوبة.</t>
+  </si>
+  <si>
+    <t>كل شيء يقترب، وكل قلق يوشك أن يزول.</t>
+  </si>
+  <si>
+    <t>اعلم أن لا شيء سيبقى على حاله.</t>
+  </si>
+  <si>
+    <t>أنت لست أول شخص يخدعه سيراب.</t>
+  </si>
+  <si>
+    <t>لا تضيع الحقوق وراء الطلبات.</t>
+  </si>
+  <si>
+    <t>من وثق بنفسه لا يحتاج إلى مدح الناس إيّاه، ومن طلب الثّناء فقد دلّ على ارتيابه في قيمة نفسه.</t>
+  </si>
+  <si>
+    <t>إذا مدح الرجل نفسه ذهب بهاؤه.</t>
+  </si>
+  <si>
+    <t>أحسن المدح أصدقه.</t>
+  </si>
+  <si>
+    <t>للمديح والملفوف طعم لذيذ، لكنّهما يسبّبان الانتفاخ.</t>
+  </si>
+  <si>
+    <t>لا تمدح النّهار قبل غروبه.</t>
+  </si>
+  <si>
+    <t>مهما وصلت إليه من نجاح وتألّق لا تكرّر كلمات المدح الرنّانة لنفسك، لا تقل "أنا أملك مقوّمات التّميّز، وأنا أختلف عن الآخرين، ولا أقارن بشخص غيري"، بل اكتفِ بالرّضا المقبول عن نفسك، وحاول أن يصل الألق إلى روحك، واصنع لك مجداً بداخلك عنوانه السّلام، بعيداً عن مبدأ المنافسة وفكرة إثبات الذات.</t>
+  </si>
+  <si>
+    <t>في زمن يُكثر فيه العاديون من مدح أنفسهم ويبالغوا في ذلك فما ظنّك بالخارقين.</t>
+  </si>
+  <si>
+    <t>إذا مدحك واحد بما ليس فيك فلا تأمن أن يذمّك أيضاً بما ليس فيك.</t>
+  </si>
+  <si>
+    <t>نحن نحبّ أحياناً حتّى المدائح الّتي لا نعتقد أنّها صادقة.</t>
+  </si>
+  <si>
+    <t>من يعرف كيف يمدح يعرف كيف يشتم.</t>
+  </si>
+  <si>
+    <t>لا يجتمع الإخلاص في القلب، ومحبّة المدح والثّناء.</t>
+  </si>
+  <si>
+    <t>Good Moral: مُحِبّ</t>
+  </si>
+  <si>
+    <t>الشّيء الّذي لا يحسن أن يقال، وإن كان حقَّاً، مدح الإنسان نفسه.</t>
+  </si>
+  <si>
+    <t>من يمدح العروس سوى أهلها.</t>
+  </si>
+  <si>
+    <t>في المديح بداية الشّتيمة.</t>
+  </si>
+  <si>
+    <t>من مدحك فإنّما مدح مواهب الله عندك، فالفضل لمن منحك لا لمن مدحك.</t>
+  </si>
+  <si>
+    <t>إذا قبلت مديحاً وقد أتيت قبيحاً، فقد قبلت هجاء مصرّحاً تصريحاً.</t>
+  </si>
+  <si>
+    <t>إذا مدحتم فلا تطيلوا المادحة؛ فإنّه يُنسى أوّلها ولا يُحفظ آخرها، وإذا هجوتم فخالفوا.</t>
+  </si>
+  <si>
+    <t>لا تمدح النّهار قبل غروبه، ولا المرأة قبل موتها.</t>
+  </si>
+  <si>
+    <t>المديح الحقيقي هو الّذي يقوله فيك عدوّك.</t>
+  </si>
+  <si>
+    <t>امدح الإنسان بعد موته.</t>
+  </si>
+  <si>
+    <t>المديح الكاذب يفضّل على النّقد الصّادق.</t>
+  </si>
+  <si>
+    <t>المدح غير المستحقّ، سخرية متخفّية.</t>
+  </si>
+  <si>
+    <t>الأمور الّتي تعرفها تعادل في حجمها حفنة الرّمل الّتي في يدك، أمّا الأمور التي لا تعرفها تعادل في حجمها حجم الكون.</t>
+  </si>
+  <si>
+    <t>المدح بعد الحياة حياة.</t>
+  </si>
+  <si>
+    <t>من مدحك بما ليس فيك وهو راض عنك، ذمّك بما ليس فيك وهو ساخط عليك.</t>
+  </si>
+  <si>
+    <t>كلمات الثّناء لا توفيك حقّك، شكراً لك على عطائك المميز، وحملك الأمانة بكل إخلاص، في عهدك كانت النّقابة في أفضل مراتبها، ولولا جهودكم لما كان للنّجاح أيّ وصول ولما تحقّقت الأهداف، فقد كنت أساس رفعة وتقدّم.</t>
+  </si>
+  <si>
+    <t>Good Moral: الأمانة</t>
+  </si>
+  <si>
+    <t>وحلف الوفاء يميناً أن يقاسمك الوفاء، دمت بخير يا واحداً ليس له مثيل.</t>
+  </si>
+  <si>
+    <t>Good Moral: وَفاء</t>
+  </si>
+  <si>
+    <t>يعجز اللّسان عن الثّناء، فلك منّي عظيم الودّ والتّقدير، لقد أتعبت أهل الوصل من بعدك، فأدامك الله يا أغلى من عرفت.</t>
+  </si>
+  <si>
+    <t>كلمات الشّكر لن توافيك، أخي والله إنّ اللّسان يعجز عن مدحك، والأحرف تعجز عن التّعبير لك حفظك الله.</t>
+  </si>
+  <si>
+    <t>تلوح في سمائنا دوماً نجوم برّاقة، لا يخفت بريقها عنّا لحظةً واحدةً، نترقّب إضاءتها بقلوب ولهانة، ونسعد بلمعانها في سمائنا كلّ ساعة، فقد استحقّت وبكلّ فخر أن يُرفع اسمها في عليانا.</t>
+  </si>
+  <si>
+    <t>عبر نفحات النّسيم وأريج الأزاهير وخيوط الأصيل، أرسل شكراً من الأعماق لك.</t>
+  </si>
+  <si>
+    <t>من أيّ أبواب الثّناء سندخل، وبأيّ أبيات القصيد نعبّر، وفي كلّ لمسة من جودكم وأكفكّم للمكرمات أسطر، كنت كسحابة معطاءة سقت الأرض فاخضرّت، كنت ولا زلت كالنّخلة الشّامخة تعطي بلا حدود، فجزاك عنّا أفضل ما جزى العاملين المخلصين، وبارك الله لك وأسعدك أينما حطّت بك الرّحال.</t>
+  </si>
+  <si>
+    <t>بكلّ الحبّ والوفاء، وبأرقّ كلمات المدح والثّناء، ومن قلوب ملؤها الإخاء، نتقدّم بالشّكر لمن تفانت في عملها.</t>
+  </si>
+  <si>
+    <t>إليك يا من كان لها قَدَم السّبق في ركب العلم والتّعليم، إليك يا من بذلتِ ولم تنتظري العطاء، إليك أُهدي عبارات الشّكر والتّقدير.</t>
+  </si>
+  <si>
+    <t>تتسابق الكلمات وتتزاحم العبارات لتنظم عقد الشّكر الّذي لا يستحقّه إلّا أنت.</t>
+  </si>
+  <si>
+    <t>إليكِ يا من كان لها قدم السّبق في ركب العلم والتّعليم، إليك يا بذلتِ ولم تنتظري العطاء، إليك أهدي عبارات الشّكر والتّقدير.</t>
+  </si>
+  <si>
+    <t>لقد أخطأت في مدحي كما أخطأت في منعي لقد أنزلت حاجاتي بواد غير ذي زرع.</t>
+  </si>
+  <si>
+    <t>ربّ مدح أذاع في النّاس فضلاً وأتاهم بقدوة ومثالِ وثناء على فتى عمّ قوماً قيمة العقد حسن اللآلي</t>
+  </si>
+  <si>
+    <t>کأنّي إذ نزلت على المعلّى نزلت على البواذخ من شمام فما ملك العراق على المعلّى بمقتدر، ولا ملك الشآم أقر حشا امرئ القيس بن حجر بنو تيم مصابيح الظلام</t>
+  </si>
+  <si>
+    <t>تحْمِلُه النّاقةُ الأَدْماءُ مُعتَجِرًا بالبُردِ كالبَدْرِ جَلّى لَيلةَ الظُّلَمِ وفِي عِطَافَيْهِ أوْ أثْنَاءِ بُرْدَتِهِ ما يَعلمُ اللهُ مِن دِينٍ ومِن كَرَمِ</t>
+  </si>
+  <si>
+    <t>كَفى بِكَ داءً أَن تَرى المَوتَ شافِيا وَحَسبُ المَنايا أَن يَكُنَّ أَمانِيا تَمَنَّيتَها لَمّا تَمَنَّيتَ أَن تَرى صَديقًا فَأَعيا أَو عَدُوًّا مُداجِيا إِذا كُنتَ تَرضى أَن تَعيشَ بِذِلَّةٍ فَلا تَستَعِدَّنَّ الحُسامَ اليَمانِيا وَلا تَستَطيلَنَّ الرِماحَ لِغارَةٍ وَلا تَستَجيدَنَّ العِتاقَ المَذاكِيا</t>
+  </si>
+  <si>
+    <t>كلُّ امرىءٍ مدح امرأً لنواله فأطال فيه فقد أراد هجاءَهُ لو لم يقدِّر فيه بُعْدَ المُسْتقَى عند الورود لَمَا أطال رشاءَهُ غيري فإنّي لا أطيل مدائحي إلّا لأوفي من مدحتُ ثناءَهُ وأَعُدُّ ظلماً أن أُقِلَّ مديحَهُ عمداً وأَسخطُ أنْ يُقِلَّ عطاءَهُ</t>
+  </si>
+  <si>
+    <t>الطَّاهِرُونَ كَأَنَّهمْ مَاءُ السَّمَا لَم يَلْتَصِقْ دَرَنٌ بِهِمْ وَعُيُوبُ إِنَّا وَقَد جُزْنَا المَدَى وَتَقَارَبَتْ آجالُنَا وأَمَضَّنَا التَّجرِيبُ وَتَحَالَفَتْ أَطوَارُنا وَتَمازَجَتْ وَنَبا بِنَا التَّقرِيعُ وَالتَّأنِيبُ وَتَخاذَلَتْ خُطواتُنا من فَرْط ما جَدَّ السُّرَى، وَالشَّدُّ، وَالتَقرِيبُ لِنَراكُمُ المَثَلَ العَلِيَّ لأمّةٍ تَرمِي إِلى أَهدَافِهَا وَتُصيب</t>
+  </si>
+  <si>
+    <t>قَرَّت عُيونُ المَجدِ وَالفَخرِ بِخِلعَةِ الشَمسِ عَلى البَدرِ صَبَّت عَلى عِطفَيهِ أَطرافَها مُعلَمَةً بِالعِزِّ وَالنَصرِ كَأَنَّها خِلعَةُ ثَوبِ الدُّجى في عاتِقِ العَيّوقِ وَالنَسرِ زَرَّ عَلَيهِ المَلكُ فَضفاضَها وَإِنَّما زَرَّ عَلى النَسرِ خَطَوتَ فيها غَيرَ مُستَكبِرٍ خَطوَ السُّها في خِلَعِ الفَجرِ</t>
+  </si>
+  <si>
+    <t>عَلى قَدرِ أَهلِ العَزمِ تَأتي العَزائِمُ وَتَأتي عَلى قَدرِ الكِرامِ المَكارِمُ وَتَعظُمُ في عَينِ الصَغيرِ صِغارُها وَتَصغُرُ في عَينِ العَظيمِ العَظائِمُ يُكَلِّفُ سَيفُ الدَولَةِ الجَيشَ هَمَّهُ وَقَد عَجَزَت عَنهُ الجُيوشُ الخَضارِمُ وَيَطلِبُ عِندَ الناسِ ما عِندَ نَفسِهِ وَذَلِكَ ما لا تَدَّعيهِ الضَراغِم يُفَدّي أَتَمُّ الطَيرِ عُمرًا سِلاحُه نُسورُ المَلا أَحداثُها وَالقَشاعِمُ</t>
+  </si>
+  <si>
+    <t>فَخَرتُم بِاللِّواءِ وَشَرُّ فَخرٍ لِواءٌ حينَ رُدَّ إِلى صُؤابِ جَعَلتُم فَخرَكُم فيهِ لِعَبدٍ مِنَ اِلأَمِ مَن يَطا عَفَرَ التُرابِ حَسِبتُم وَالسَفيهُ أَخو ظُنونٍ وَذَلِكَ لَيسَ مِن أَمرِ الصَوابِ بِأَنَّ لِقاءَنا إِذ حانَ يَومٌ بِمَكَّةَ بَيعُكُم حُمرَ الثِيابِ أَقَرَّ العَينَ أَن عُصِبَت يَداهُ وَما إِن تُعصَبانِ عَلى خِضابِ</t>
+  </si>
+  <si>
+    <t>إن قلت شكراً فشكري لن يوفيكم حقَّاً سعيتم فكان السّعي مشكوراً إن جفّ حبري عن التّعبير يكتبكم قلب به من صفاء الحبّ تعبيراً.</t>
+  </si>
+  <si>
+    <t>يهوى الثّناء مبرِّز ومقصِّر حبّ الثّناء طبيعة الإنسان.</t>
+  </si>
+  <si>
+    <t>إذا المرء لم يمدحه حسن فعاله فمادحه يهذي وإن كان مفصحاً.</t>
+  </si>
+  <si>
+    <t>ثلاث موبقات هي: الكبر فإنه حط إبليس من مرتبته، والحرص فإنه أخرج آدم من الجنة، والحسد فإنه دعا ابن آدم إلى قتل أخيه.</t>
+  </si>
+  <si>
+    <t>Blameworthy Moral: كُبْر</t>
+  </si>
+  <si>
+    <t>الحسد إهانة للذات.</t>
+  </si>
+  <si>
+    <t>الحسد هو عد النعم التي يحظى بها الآخرون بدلاً من عد نعمك.</t>
+  </si>
+  <si>
+    <t>الحاسد يصوّب على الآخرين ويجرح نفسه.</t>
+  </si>
+  <si>
+    <t>الحسد مثل النار دائماً تستهدف أعلى النقاط.</t>
+  </si>
+  <si>
+    <t>ليس الحاسد هو الذي يطمع أن يساويك بأن يرقى إليك، بل هو الذي يريد أن تساويه بأن تنزل إليه.</t>
+  </si>
+  <si>
+    <t>ما يثير في الناس الحسد ما لا يستطيعون هم أنفسهم أن يتمتعوا به.</t>
+  </si>
+  <si>
+    <t>قبل أن يبدأ الإنسان حياته عليه أن يقاتل شعور الحسد والكراهية في نفسه.</t>
+  </si>
+  <si>
+    <t>الحسد أغبى الرذائل إطلاقاً، فإنه لا يعود على صاحبه بأية فائدة.</t>
+  </si>
+  <si>
+    <t>يمكنني أن أرضي الناس كلهم إلا حاسد نعمة، فإنه لا يرضيه إلا زوالها.</t>
+  </si>
+  <si>
+    <t>لا يمكنك أن تكون سعيداً وحاسداً بنفس الوقت.</t>
+  </si>
+  <si>
+    <t>اصبر على كيد الحسود فإن صبرك قاتله، كالنار تأكل بعضها إن لم تجد ما تأكله.</t>
+  </si>
+  <si>
+    <t>لله در الحسد ما أعدله، بدأ بصاحبه فقتله.</t>
+  </si>
+  <si>
+    <t>الحسد أول خطيئة ظهرت في السموات، وأول معصية حدثت في الأرض.</t>
+  </si>
+  <si>
+    <t>إن الحسد في دين المسلم أسرع من الآكلة في جسده.</t>
+  </si>
+  <si>
+    <t>يأكل الحسد الحاسدين كما يأكل الصدأ الحديد.</t>
+  </si>
+  <si>
+    <t>كن سعيداً كلما كثر حسادك فهم الشهادة لك على نجاحك.</t>
+  </si>
+  <si>
+    <t>مسكين هو الحاسد لا يظلم إلا نفسه.</t>
+  </si>
+  <si>
+    <t>الحسد عاطفة مفعمة بالجبن والعار بحيث لا يجرؤ إنسان على الاعتراف بها.</t>
+  </si>
+  <si>
+    <t>ما يلقاه الرجل من حسد أقرانه أشد مما يلقاه من كيد أعدائه.</t>
+  </si>
+  <si>
+    <t>الحسد ينبع من انعدام الثقة، لا بالآخرين بل بالذات.</t>
+  </si>
+  <si>
+    <t>الأنانية تولّد الحسد، والحسد يولّد البغضاء، والبغضاء تولّد الاختلاف، والاختلاف يولّد الفرقة، والفرقة تولد الضعف، والضعف يولّد الذل، والذل يولّد زوال الدولة، وزوال النعمة، وهلاك الأمة.</t>
+  </si>
+  <si>
+    <t>الحسد يأكل المودة، والجحود لا يفسد الود وحده، ولكنه يفسد المروءة أيضاً.</t>
+  </si>
+  <si>
+    <t>الحاسد مغتاظ على من لا ذنب له، ويبخل بما لا يملكه، ويطلب ما لا يجده.</t>
+  </si>
+  <si>
+    <t>لا نحسد إلا أولئك الذين نعرفهم جيداً، ونخالطهم كثيراً، والذين من المفروض أن نفرح لنجاحهم لهذا يوجد شيء ما حقير في كل صداقة ولهذا لا نحب أقرباءنا إلّا في الحالة التي يكونون فيها ضحايا.</t>
+  </si>
+  <si>
+    <t>لا يحمل الحقد من تعلو به الرتب، ولا ينال العلا من طبعه الغضب.</t>
+  </si>
+  <si>
+    <t>المؤمن يغبط ولا يحسد، والغبطة من الإيمان، والحسد من النفاق.</t>
+  </si>
+  <si>
+    <t>لون الحاسد شاحب وكلامه نميمة، ومهما ر الزمن سيبقى الحاسد حاقدا، لا ترجى مودته.</t>
+  </si>
+  <si>
+    <t>Blameworthy Moral: نَمِيم</t>
+  </si>
+  <si>
+    <t>متى دخل الحسد والغيرة خرجت الحقيقة من الرأس.</t>
+  </si>
+  <si>
+    <t>كنت أحسد من له حذاء إلى أن رأيت رجلاً بلا قدمين.</t>
+  </si>
+  <si>
+    <t>الموت يفتح باب الشهرة ويغلق باب الحسد.</t>
+  </si>
+  <si>
+    <t>نحتاج إلى أن نغسل قلوبنا كل يوم من كل شعور بسيط وصغير بالحسد لأي إنسان، مهما صعبت ظروفنا ومهما قهرنا الحرمان علينا أن ندرك أن الكمال غير موجود وأن الحسد جهل، فلا أحد كامل بشكل يستحق الحسد، فما يكسبه في يد يفقده من يد أخرى، مثلنا تماما نفقد بعض رغباتنا ونحرم منها، لكننا في اليد الأخرى نمتلك كثيرا من الرغبات التي يتمناها الآخرون ويحلمون بها</t>
+  </si>
+  <si>
+    <t>أشعر كأن كل حلم من أحلامي وأمنية من أمنياتي قد خرجت من نفسي وصعدت إلى السماء فشُذبت ورُتبت وعُدلت وصيغت في حال أطهر ثم أُعيدت إلى صدري مرة أخرى، لأن الأحلام يا أخي إذا تأخرت في صدرك تفسد، وإذا باتت في نفسك سنة بعد سنة تشوبها الشوائب وتتراكم فوقها أتربة من الأنانية والحسد واليأس، رضا الله يخلقك مرةً أخرى بقلب جديد وأحلام نظيفة.</t>
+  </si>
+  <si>
+    <t>كثيراً ما يخطئ الناس في الظن بأن التواضع يقهر الكبرياء ويطفئ أحقاد الحساد .. هناك حالات عدة، لا يجدي التواضع فيها فتيلاً، ويكون فيها بالإضافة إلى ذلك عائقاً ولا سيما عندما يستخدم في التعامل مع أناس متغطرسين، قد يدفعهم الحسد أو أي شيء آخر إلى حمل الكراهية لك.</t>
+  </si>
+  <si>
+    <t>يكمن الحسد في جذر خوفنا الوجودي، انظر إلى تاريخ بني آدم، كل تلك الحروب وذاك الخراب، هل تعرفون ما الذي قالوه عندما توقفت الحرب العالمية الأولى؟ قالوا إنّها الحرب التي ستنهي كل الحروب! وبالطبع لم يحدث ذلك، فالإنسان حسود بطبعه، وأنانيته تدفعه إلى الأذى وحسده يقوي الصراع لم تنته الحروب لأنّ هناك ظلمًا وتفرقة، وبدلًا من الاشتغال بحل ذلك، أنتجنا عرقية ودينية ونحن الآن موعودون بمزيد من التعارضات التي لم نعرف لها مثيلًا في التاريخ.</t>
+  </si>
+  <si>
+    <t>جاملْ عدوَّك ما استطعتَ فإنَّه جاملْ عدوَّك ما استطعتَ فإنَّه بالرفقِ يطمع في صلاح الفاسدِ بالرفقِ يطمع في صلاح الفاسدِ واحذرْ حسودَك ما استطعت فإنَّه واحذرْ حسودَك ما استطعت فإنَّه إن نمت عنه فليس عنك براقدِ إن نمت عنه فليس عنك براقدِ إنَّ الحسودَ وإن أراك توددًا إنَّ الحسودَ وإن أراك توددًا منه أضرُّ من العدو الحاقدِ منه أضرُّ من العدو الحاقدِ ولربما رضي العدوُّ إذا رأى ولربما رضي العدوُّ إذا رأى منك الجميلَ فصار غير معاندِ منك الجميلَ فصار غير معاندِ ورضا الحسودِ زوالُ نعمتك التي ورضا الحسودِ زوالُ نعمتك التي أوتيتها من طارف أو تالدِ أوتيتها من طارف أو تالدِ فاصبرْ على غيظِ الحسود فنارُه فاصبرْ على غيظِ الحسود فنارُه ترمي حشاه بالعذابِ الخالدِ ترمي حشاه بالعذابِ الخالدِ تضفو على المحسودِ نعمةُ ربِّه تضفو على المحسودِ نعمةُ ربِّه ويذوبُ من كمدٍ فؤادُ الحاسدِ ويذوبُ من كمدٍ فؤادُ الحاسدِ</t>
+  </si>
+  <si>
+    <t>حسدوا الفتى إذ لم ينالوا سعيَه حسدوا الفتى إذ لم ينالوا سعيَه فالقومُ أعداءٌ له وخصومُ فالقومُ أعداءٌ له وخصومُ كضرائرِ الحسناءِ قلنَ لوجهِها كضرائرِ الحسناءِ قلنَ لوجهِها حسدًا وبغيًا إنَّه لدميمُ حسدًا وبغيًا إنَّه لدميمُ والوجهُ يشرقُ في الظلامِ كأنَّه والوجهُ يشرقُ في الظلامِ كأنَّه بدرٌ منيرٌ والنساءُ نجومُ بدرٌ منيرٌ والنساءُ نجومُ وترَى اللبيبَ محسدًا لم يجترمْ وترَى اللبيبَ محسدًا لم يجترمْ شتمَ الرجالِ وعرضُه مشتومُ شتمَ الرجالِ وعرضُه مشتومُ وكذاك مَن عظمتْ عليه نعمةٌ وكذاك مَن عظمتْ عليه نعمةٌ حسادُه سيفٌ عليه صرومُ حسادُه سيفٌ عليه صرومُ فاتركْ محاورةَ السفيهِ فإنَّها فاتركْ محاورةَ السفيهِ فإنَّها ندمٌ وغبٌّ بعدَ ذاك وخيمُ ندمٌ وغبٌّ بعدَ ذاك وخيمُ</t>
+  </si>
+  <si>
+    <t>لمنْ جاهدَ الحُسَّادَ أجرُ المجاهدِ، وأعجَزُ مَا حَاوَلتُ إرْضَاءُ حَاسِدِ ولمْ أرَ مثلي اليومَ أكثرُ حاسداً كأنَّ قُلُوبَ النَّاسِ لي قَلبُ وَاجِدِ ألمْ يَرَ هذا النّاسُ غَيْرِيَ فاضِلاً؟ ولمْ يَظْفَرِ الحُسَّادُ قَبلي بمَاجِدِ؟! أرى الغلَّ مِنْ تحتِ النفاقِ وأجتني مِنَ العَسَلِ المَاذِيّ سُمّ الأسَاوِدِ وَأصْبِرُ مَا لْم يُحْسَبِ الصَّبْرُ ذِلّةً، وَألْبَسُ للمَذْمُومِ حُلّة حَامِدِ</t>
+  </si>
+  <si>
+    <t>ألا إنَّ أخلاقَ الفَتَى كزَمانِهِ، فمنهُنَّ بِيضٌ في العيون وسُودُ وتأكُلنا أيَّامُنا فكأنَّما تَمرُّ بِنا السَّاعاتُ وهي أُسودُ وقد يَخمُلُ الإنسانُ في عُنفوانِه وينبَهُ مِن بَعدِ النُّهَى فيسودُ فلا تحسُدنَّ يوماً على فضلِ نعمةٍ، فحسبُكَ عَاراً أنْ يُقالَ حَسودُ</t>
+  </si>
+  <si>
+    <t>Good Moral: آلِف</t>
+  </si>
+  <si>
+    <t>إن شئت قتل الحاسدين تعمدا من غير عادية عليك ولا قود وبغير سم قاتل وصوارم وعقاب رب ليس يغفل عن أحد عظم تجاه عيونهم محسودهم فتراهم موتى النفوس مع الجسد ذوب المعادن باللظى لكنما ذوب الحسود بحر نيران الحسد لم يبلغ الحساد أجالا لهم إذ أنهم سماهم موت الكمد حد الزناة من الشريعة مدة وترى الحسود بدائه أبدا يحد</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -746,25 +1423,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -802,7 +1471,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -836,7 +1505,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -871,10 +1539,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1047,17 +1714,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B205"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B428"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1065,7 +1729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1073,7 +1737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1081,7 +1745,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1089,7 +1753,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1097,7 +1761,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1105,7 +1769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1113,7 +1777,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1121,7 +1785,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1129,7 +1793,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1137,7 +1801,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1145,7 +1809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1153,7 +1817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1161,7 +1825,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1169,7 +1833,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1177,7 +1841,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1185,7 +1849,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1193,7 +1857,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1201,7 +1865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1209,7 +1873,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1217,7 +1881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1225,7 +1889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1233,7 +1897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1241,7 +1905,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1249,7 +1913,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1257,7 +1921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1265,7 +1929,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1273,7 +1937,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1281,7 +1945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1289,7 +1953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1297,7 +1961,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -1305,7 +1969,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1313,7 +1977,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -1321,7 +1985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -1329,7 +1993,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -1337,7 +2001,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -1345,7 +2009,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -1353,7 +2017,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -1361,7 +2025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -1369,7 +2033,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -1377,7 +2041,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>51</v>
       </c>
@@ -1385,7 +2049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -1393,7 +2057,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>53</v>
       </c>
@@ -1401,7 +2065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>54</v>
       </c>
@@ -1409,7 +2073,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -1417,7 +2081,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -1425,7 +2089,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>59</v>
       </c>
@@ -1433,7 +2097,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>61</v>
       </c>
@@ -1441,7 +2105,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>62</v>
       </c>
@@ -1449,7 +2113,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -1457,7 +2121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>64</v>
       </c>
@@ -1465,7 +2129,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>65</v>
       </c>
@@ -1473,7 +2137,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>67</v>
       </c>
@@ -1481,7 +2145,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>69</v>
       </c>
@@ -1489,7 +2153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>70</v>
       </c>
@@ -1497,7 +2161,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>71</v>
       </c>
@@ -1505,7 +2169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>72</v>
       </c>
@@ -1513,7 +2177,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>73</v>
       </c>
@@ -1521,7 +2185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -1529,7 +2193,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>75</v>
       </c>
@@ -1537,7 +2201,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>76</v>
       </c>
@@ -1545,7 +2209,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>77</v>
       </c>
@@ -1553,7 +2217,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>78</v>
       </c>
@@ -1561,7 +2225,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2">
       <c r="A64" t="s">
         <v>79</v>
       </c>
@@ -1569,7 +2233,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2">
       <c r="A65" t="s">
         <v>80</v>
       </c>
@@ -1577,7 +2241,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2">
       <c r="A66" t="s">
         <v>81</v>
       </c>
@@ -1585,7 +2249,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2">
       <c r="A67" t="s">
         <v>82</v>
       </c>
@@ -1593,7 +2257,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2">
       <c r="A68" t="s">
         <v>83</v>
       </c>
@@ -1601,7 +2265,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2">
       <c r="A69" t="s">
         <v>84</v>
       </c>
@@ -1609,7 +2273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2">
       <c r="A70" t="s">
         <v>85</v>
       </c>
@@ -1617,7 +2281,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2">
       <c r="A71" t="s">
         <v>86</v>
       </c>
@@ -1625,7 +2289,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2">
       <c r="A72" t="s">
         <v>87</v>
       </c>
@@ -1633,7 +2297,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2">
       <c r="A73" t="s">
         <v>88</v>
       </c>
@@ -1641,7 +2305,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2">
       <c r="A74" t="s">
         <v>89</v>
       </c>
@@ -1649,7 +2313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2">
       <c r="A75" t="s">
         <v>90</v>
       </c>
@@ -1657,7 +2321,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2">
       <c r="A76" t="s">
         <v>91</v>
       </c>
@@ -1665,7 +2329,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2">
       <c r="A77" t="s">
         <v>92</v>
       </c>
@@ -1673,7 +2337,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2">
       <c r="A78" t="s">
         <v>93</v>
       </c>
@@ -1681,7 +2345,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2">
       <c r="A79" t="s">
         <v>94</v>
       </c>
@@ -1689,7 +2353,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2">
       <c r="A80" t="s">
         <v>95</v>
       </c>
@@ -1697,7 +2361,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2">
       <c r="A81" t="s">
         <v>96</v>
       </c>
@@ -1705,7 +2369,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2">
       <c r="A82" t="s">
         <v>97</v>
       </c>
@@ -1713,7 +2377,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2">
       <c r="A83" t="s">
         <v>98</v>
       </c>
@@ -1721,7 +2385,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2">
       <c r="A84" t="s">
         <v>99</v>
       </c>
@@ -1729,7 +2393,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2">
       <c r="A85" t="s">
         <v>100</v>
       </c>
@@ -1737,7 +2401,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2">
       <c r="A86" t="s">
         <v>4</v>
       </c>
@@ -1745,7 +2409,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2">
       <c r="A87" t="s">
         <v>101</v>
       </c>
@@ -1753,7 +2417,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2">
       <c r="A88" t="s">
         <v>102</v>
       </c>
@@ -1761,7 +2425,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2">
       <c r="A89" t="s">
         <v>103</v>
       </c>
@@ -1769,7 +2433,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2">
       <c r="A90" t="s">
         <v>104</v>
       </c>
@@ -1777,7 +2441,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2">
       <c r="A91" t="s">
         <v>106</v>
       </c>
@@ -1785,7 +2449,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2">
       <c r="A92" t="s">
         <v>107</v>
       </c>
@@ -1793,7 +2457,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2">
       <c r="A93" t="s">
         <v>108</v>
       </c>
@@ -1801,7 +2465,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2">
       <c r="A94" t="s">
         <v>109</v>
       </c>
@@ -1809,7 +2473,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2">
       <c r="A95" t="s">
         <v>110</v>
       </c>
@@ -1817,7 +2481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2">
       <c r="A96" t="s">
         <v>111</v>
       </c>
@@ -1825,7 +2489,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2">
       <c r="A97" t="s">
         <v>112</v>
       </c>
@@ -1833,7 +2497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2">
       <c r="A98" t="s">
         <v>113</v>
       </c>
@@ -1841,7 +2505,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2">
       <c r="A99" t="s">
         <v>114</v>
       </c>
@@ -1849,7 +2513,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2">
       <c r="A100" t="s">
         <v>115</v>
       </c>
@@ -1857,7 +2521,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2">
       <c r="A101" t="s">
         <v>116</v>
       </c>
@@ -1865,7 +2529,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2">
       <c r="A102" t="s">
         <v>117</v>
       </c>
@@ -1873,7 +2537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2">
       <c r="A103" t="s">
         <v>118</v>
       </c>
@@ -1881,7 +2545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2">
       <c r="A104" t="s">
         <v>119</v>
       </c>
@@ -1889,7 +2553,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2">
       <c r="A105" t="s">
         <v>120</v>
       </c>
@@ -1897,7 +2561,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2">
       <c r="A106" t="s">
         <v>122</v>
       </c>
@@ -1905,7 +2569,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2">
       <c r="A107" t="s">
         <v>123</v>
       </c>
@@ -1913,7 +2577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2">
       <c r="A108" t="s">
         <v>124</v>
       </c>
@@ -1921,7 +2585,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2">
       <c r="A109" t="s">
         <v>125</v>
       </c>
@@ -1929,7 +2593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2">
       <c r="A110" t="s">
         <v>126</v>
       </c>
@@ -1937,7 +2601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2">
       <c r="A111" t="s">
         <v>127</v>
       </c>
@@ -1945,7 +2609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2">
       <c r="A112" t="s">
         <v>128</v>
       </c>
@@ -1953,7 +2617,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2">
       <c r="A113" t="s">
         <v>129</v>
       </c>
@@ -1961,7 +2625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2">
       <c r="A114" t="s">
         <v>130</v>
       </c>
@@ -1969,7 +2633,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2">
       <c r="A115" t="s">
         <v>131</v>
       </c>
@@ -1977,7 +2641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2">
       <c r="A116" t="s">
         <v>132</v>
       </c>
@@ -1985,7 +2649,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2">
       <c r="A117" t="s">
         <v>133</v>
       </c>
@@ -1993,7 +2657,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2">
       <c r="A118" t="s">
         <v>134</v>
       </c>
@@ -2001,7 +2665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2">
       <c r="A119" t="s">
         <v>135</v>
       </c>
@@ -2009,7 +2673,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2">
       <c r="A120" t="s">
         <v>136</v>
       </c>
@@ -2017,7 +2681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2">
       <c r="A121" t="s">
         <v>137</v>
       </c>
@@ -2025,7 +2689,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2">
       <c r="A122" t="s">
         <v>138</v>
       </c>
@@ -2033,7 +2697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2">
       <c r="A123" t="s">
         <v>139</v>
       </c>
@@ -2041,7 +2705,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2">
       <c r="A124" t="s">
         <v>140</v>
       </c>
@@ -2049,7 +2713,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2">
       <c r="A125" t="s">
         <v>141</v>
       </c>
@@ -2057,7 +2721,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2">
       <c r="A126" t="s">
         <v>142</v>
       </c>
@@ -2065,7 +2729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2">
       <c r="A127" t="s">
         <v>143</v>
       </c>
@@ -2073,7 +2737,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2">
       <c r="A128" t="s">
         <v>144</v>
       </c>
@@ -2081,7 +2745,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2">
       <c r="A129" t="s">
         <v>145</v>
       </c>
@@ -2089,7 +2753,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2">
       <c r="A130" t="s">
         <v>147</v>
       </c>
@@ -2097,7 +2761,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2">
       <c r="A131" t="s">
         <v>148</v>
       </c>
@@ -2105,7 +2769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2">
       <c r="A132" t="s">
         <v>149</v>
       </c>
@@ -2113,7 +2777,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2">
       <c r="A133" t="s">
         <v>151</v>
       </c>
@@ -2121,7 +2785,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2">
       <c r="A134" t="s">
         <v>152</v>
       </c>
@@ -2129,7 +2793,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2">
       <c r="A135" t="s">
         <v>153</v>
       </c>
@@ -2137,7 +2801,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2">
       <c r="A136" t="s">
         <v>154</v>
       </c>
@@ -2145,7 +2809,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2">
       <c r="A137" t="s">
         <v>155</v>
       </c>
@@ -2153,7 +2817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2">
       <c r="A138" t="s">
         <v>156</v>
       </c>
@@ -2161,7 +2825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2">
       <c r="A139" t="s">
         <v>157</v>
       </c>
@@ -2169,7 +2833,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2">
       <c r="A140" t="s">
         <v>158</v>
       </c>
@@ -2177,7 +2841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2">
       <c r="A141" t="s">
         <v>159</v>
       </c>
@@ -2185,7 +2849,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2">
       <c r="A142" t="s">
         <v>160</v>
       </c>
@@ -2193,7 +2857,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:2">
       <c r="A143" t="s">
         <v>161</v>
       </c>
@@ -2201,7 +2865,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2">
       <c r="A144" t="s">
         <v>163</v>
       </c>
@@ -2209,7 +2873,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:2">
       <c r="A145" t="s">
         <v>164</v>
       </c>
@@ -2217,7 +2881,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:2">
       <c r="A146" t="s">
         <v>165</v>
       </c>
@@ -2225,7 +2889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:2">
       <c r="A147" t="s">
         <v>166</v>
       </c>
@@ -2233,7 +2897,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:2">
       <c r="A148" t="s">
         <v>167</v>
       </c>
@@ -2241,7 +2905,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:2">
       <c r="A149" t="s">
         <v>168</v>
       </c>
@@ -2249,7 +2913,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:2">
       <c r="A150" t="s">
         <v>169</v>
       </c>
@@ -2257,7 +2921,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:2">
       <c r="A151" t="s">
         <v>171</v>
       </c>
@@ -2265,7 +2929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:2">
       <c r="A152" t="s">
         <v>172</v>
       </c>
@@ -2273,7 +2937,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:2">
       <c r="A153" t="s">
         <v>173</v>
       </c>
@@ -2281,7 +2945,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:2">
       <c r="A154" t="s">
         <v>175</v>
       </c>
@@ -2289,7 +2953,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:2">
       <c r="A155" t="s">
         <v>176</v>
       </c>
@@ -2297,7 +2961,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:2">
       <c r="A156" t="s">
         <v>177</v>
       </c>
@@ -2305,7 +2969,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:2">
       <c r="A157" t="s">
         <v>178</v>
       </c>
@@ -2313,7 +2977,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:2">
       <c r="A158" t="s">
         <v>179</v>
       </c>
@@ -2321,7 +2985,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:2">
       <c r="A159" t="s">
         <v>180</v>
       </c>
@@ -2329,7 +2993,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:2">
       <c r="A160" t="s">
         <v>181</v>
       </c>
@@ -2337,7 +3001,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:2">
       <c r="A161" t="s">
         <v>182</v>
       </c>
@@ -2345,7 +3009,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:2">
       <c r="A162" t="s">
         <v>183</v>
       </c>
@@ -2353,7 +3017,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:2">
       <c r="A163" t="s">
         <v>184</v>
       </c>
@@ -2361,7 +3025,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:2">
       <c r="A164" t="s">
         <v>185</v>
       </c>
@@ -2369,7 +3033,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:2">
       <c r="A165" t="s">
         <v>186</v>
       </c>
@@ -2377,7 +3041,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:2">
       <c r="A166" t="s">
         <v>187</v>
       </c>
@@ -2385,7 +3049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:2">
       <c r="A167" t="s">
         <v>188</v>
       </c>
@@ -2393,7 +3057,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:2">
       <c r="A168" t="s">
         <v>189</v>
       </c>
@@ -2401,7 +3065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:2">
       <c r="A169" t="s">
         <v>190</v>
       </c>
@@ -2409,7 +3073,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:2">
       <c r="A170" t="s">
         <v>192</v>
       </c>
@@ -2417,7 +3081,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:2">
       <c r="A171" t="s">
         <v>193</v>
       </c>
@@ -2425,7 +3089,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:2">
       <c r="A172" t="s">
         <v>194</v>
       </c>
@@ -2433,7 +3097,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:2">
       <c r="A173" t="s">
         <v>195</v>
       </c>
@@ -2441,7 +3105,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:2">
       <c r="A174" t="s">
         <v>196</v>
       </c>
@@ -2449,7 +3113,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:2">
       <c r="A175" t="s">
         <v>197</v>
       </c>
@@ -2457,7 +3121,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:2">
       <c r="A176" t="s">
         <v>198</v>
       </c>
@@ -2465,7 +3129,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:2">
       <c r="A177" t="s">
         <v>199</v>
       </c>
@@ -2473,7 +3137,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:2">
       <c r="A178" t="s">
         <v>200</v>
       </c>
@@ -2481,7 +3145,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:2">
       <c r="A179" t="s">
         <v>201</v>
       </c>
@@ -2489,7 +3153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:2">
       <c r="A180" t="s">
         <v>202</v>
       </c>
@@ -2497,7 +3161,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:2">
       <c r="A181" t="s">
         <v>203</v>
       </c>
@@ -2505,7 +3169,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:2">
       <c r="A182" t="s">
         <v>204</v>
       </c>
@@ -2513,7 +3177,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:2">
       <c r="A183" t="s">
         <v>205</v>
       </c>
@@ -2521,7 +3185,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:2">
       <c r="A184" t="s">
         <v>206</v>
       </c>
@@ -2529,7 +3193,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:2">
       <c r="A185" t="s">
         <v>207</v>
       </c>
@@ -2537,7 +3201,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:2">
       <c r="A186" t="s">
         <v>208</v>
       </c>
@@ -2545,7 +3209,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:2">
       <c r="A187" t="s">
         <v>209</v>
       </c>
@@ -2553,7 +3217,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:2">
       <c r="A188" t="s">
         <v>210</v>
       </c>
@@ -2561,7 +3225,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:2">
       <c r="A189" t="s">
         <v>211</v>
       </c>
@@ -2569,7 +3233,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:2">
       <c r="A190" t="s">
         <v>212</v>
       </c>
@@ -2577,7 +3241,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:2">
       <c r="A191" t="s">
         <v>213</v>
       </c>
@@ -2585,7 +3249,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:2">
       <c r="A192" t="s">
         <v>214</v>
       </c>
@@ -2593,7 +3257,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:2">
       <c r="A193" t="s">
         <v>215</v>
       </c>
@@ -2601,7 +3265,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:2">
       <c r="A194" t="s">
         <v>216</v>
       </c>
@@ -2609,7 +3273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:2">
       <c r="A195" t="s">
         <v>217</v>
       </c>
@@ -2617,7 +3281,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:2">
       <c r="A196" t="s">
         <v>218</v>
       </c>
@@ -2625,7 +3289,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:2">
       <c r="A197" t="s">
         <v>219</v>
       </c>
@@ -2633,7 +3297,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:2">
       <c r="A198" t="s">
         <v>220</v>
       </c>
@@ -2641,7 +3305,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:2">
       <c r="A199" t="s">
         <v>221</v>
       </c>
@@ -2649,7 +3313,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:2">
       <c r="A200" t="s">
         <v>222</v>
       </c>
@@ -2657,7 +3321,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:2">
       <c r="A201" t="s">
         <v>224</v>
       </c>
@@ -2665,7 +3329,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:2">
       <c r="A202" t="s">
         <v>225</v>
       </c>
@@ -2673,7 +3337,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:2">
       <c r="A203" t="s">
         <v>226</v>
       </c>
@@ -2681,7 +3345,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:2">
       <c r="A204" t="s">
         <v>227</v>
       </c>
@@ -2689,12 +3353,1796 @@
         <v>19</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:2">
       <c r="A205" t="s">
         <v>228</v>
       </c>
       <c r="B205" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2">
+      <c r="A206" t="s">
+        <v>229</v>
+      </c>
+      <c r="B206" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2">
+      <c r="A207" t="s">
+        <v>231</v>
+      </c>
+      <c r="B207" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2">
+      <c r="A208" t="s">
+        <v>232</v>
+      </c>
+      <c r="B208" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2">
+      <c r="A209" t="s">
+        <v>233</v>
+      </c>
+      <c r="B209" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2">
+      <c r="A210" t="s">
+        <v>234</v>
+      </c>
+      <c r="B210" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2">
+      <c r="A211" t="s">
+        <v>235</v>
+      </c>
+      <c r="B211" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2">
+      <c r="A212" t="s">
+        <v>236</v>
+      </c>
+      <c r="B212" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2">
+      <c r="A213" t="s">
+        <v>237</v>
+      </c>
+      <c r="B213" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2">
+      <c r="A214" t="s">
+        <v>238</v>
+      </c>
+      <c r="B214" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2">
+      <c r="A215" t="s">
+        <v>239</v>
+      </c>
+      <c r="B215" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2">
+      <c r="A216" t="s">
+        <v>240</v>
+      </c>
+      <c r="B216" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2">
+      <c r="A217" t="s">
+        <v>241</v>
+      </c>
+      <c r="B217" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2">
+      <c r="A218" t="s">
+        <v>242</v>
+      </c>
+      <c r="B218" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2">
+      <c r="A219" t="s">
+        <v>243</v>
+      </c>
+      <c r="B219" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2">
+      <c r="A220" t="s">
+        <v>244</v>
+      </c>
+      <c r="B220" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2">
+      <c r="A221" t="s">
+        <v>245</v>
+      </c>
+      <c r="B221" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2">
+      <c r="A222" t="s">
+        <v>246</v>
+      </c>
+      <c r="B222" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2">
+      <c r="A223" t="s">
+        <v>247</v>
+      </c>
+      <c r="B223" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2">
+      <c r="A224" t="s">
+        <v>248</v>
+      </c>
+      <c r="B224" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2">
+      <c r="A225" t="s">
+        <v>249</v>
+      </c>
+      <c r="B225" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2">
+      <c r="A226" t="s">
+        <v>250</v>
+      </c>
+      <c r="B226" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2">
+      <c r="A227" t="s">
+        <v>251</v>
+      </c>
+      <c r="B227" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2">
+      <c r="A228" t="s">
+        <v>252</v>
+      </c>
+      <c r="B228" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2">
+      <c r="A229" t="s">
+        <v>253</v>
+      </c>
+      <c r="B229" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2">
+      <c r="A230" t="s">
+        <v>254</v>
+      </c>
+      <c r="B230" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2">
+      <c r="A231" t="s">
+        <v>255</v>
+      </c>
+      <c r="B231" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2">
+      <c r="A232" t="s">
+        <v>256</v>
+      </c>
+      <c r="B232" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2">
+      <c r="A233" t="s">
+        <v>257</v>
+      </c>
+      <c r="B233" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2">
+      <c r="A234" t="s">
+        <v>258</v>
+      </c>
+      <c r="B234" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2">
+      <c r="A235" t="s">
+        <v>259</v>
+      </c>
+      <c r="B235" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2">
+      <c r="A236" t="s">
+        <v>260</v>
+      </c>
+      <c r="B236" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2">
+      <c r="A237" t="s">
+        <v>261</v>
+      </c>
+      <c r="B237" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2">
+      <c r="A238" t="s">
+        <v>262</v>
+      </c>
+      <c r="B238" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2">
+      <c r="A239" t="s">
+        <v>263</v>
+      </c>
+      <c r="B239" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2">
+      <c r="A240" t="s">
+        <v>264</v>
+      </c>
+      <c r="B240" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2">
+      <c r="A241" t="s">
+        <v>265</v>
+      </c>
+      <c r="B241" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2">
+      <c r="A242" t="s">
+        <v>266</v>
+      </c>
+      <c r="B242" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2">
+      <c r="A243" t="s">
+        <v>267</v>
+      </c>
+      <c r="B243" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2">
+      <c r="A244" t="s">
+        <v>268</v>
+      </c>
+      <c r="B244" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2">
+      <c r="A245" t="s">
+        <v>269</v>
+      </c>
+      <c r="B245" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2">
+      <c r="A246" t="s">
+        <v>270</v>
+      </c>
+      <c r="B246" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2">
+      <c r="A247" t="s">
+        <v>271</v>
+      </c>
+      <c r="B247" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2">
+      <c r="A248" t="s">
+        <v>272</v>
+      </c>
+      <c r="B248" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2">
+      <c r="A249" t="s">
+        <v>273</v>
+      </c>
+      <c r="B249" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2">
+      <c r="A250" t="s">
+        <v>274</v>
+      </c>
+      <c r="B250" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2">
+      <c r="A251" t="s">
+        <v>275</v>
+      </c>
+      <c r="B251" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2">
+      <c r="A252" t="s">
+        <v>276</v>
+      </c>
+      <c r="B252" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2">
+      <c r="A253" t="s">
+        <v>277</v>
+      </c>
+      <c r="B253" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2">
+      <c r="A254" t="s">
+        <v>278</v>
+      </c>
+      <c r="B254" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2">
+      <c r="A255" t="s">
+        <v>279</v>
+      </c>
+      <c r="B255" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2">
+      <c r="A256" t="s">
+        <v>280</v>
+      </c>
+      <c r="B256" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2">
+      <c r="A257" t="s">
+        <v>281</v>
+      </c>
+      <c r="B257" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2">
+      <c r="A258" t="s">
+        <v>282</v>
+      </c>
+      <c r="B258" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2">
+      <c r="A259" t="s">
+        <v>283</v>
+      </c>
+      <c r="B259" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2">
+      <c r="A260" t="s">
+        <v>284</v>
+      </c>
+      <c r="B260" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2">
+      <c r="A261" t="s">
+        <v>285</v>
+      </c>
+      <c r="B261" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2">
+      <c r="A262" t="s">
+        <v>286</v>
+      </c>
+      <c r="B262" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2">
+      <c r="A263" t="s">
+        <v>287</v>
+      </c>
+      <c r="B263" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2">
+      <c r="A264" t="s">
+        <v>288</v>
+      </c>
+      <c r="B264" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2">
+      <c r="A265" t="s">
+        <v>289</v>
+      </c>
+      <c r="B265" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2">
+      <c r="A266" t="s">
+        <v>290</v>
+      </c>
+      <c r="B266" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2">
+      <c r="A267" t="s">
+        <v>291</v>
+      </c>
+      <c r="B267" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2">
+      <c r="A268" t="s">
+        <v>292</v>
+      </c>
+      <c r="B268" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2">
+      <c r="A269" t="s">
+        <v>293</v>
+      </c>
+      <c r="B269" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2">
+      <c r="A270" t="s">
+        <v>294</v>
+      </c>
+      <c r="B270" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2">
+      <c r="A271" t="s">
+        <v>295</v>
+      </c>
+      <c r="B271" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2">
+      <c r="A272" t="s">
+        <v>296</v>
+      </c>
+      <c r="B272" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2">
+      <c r="A273" t="s">
+        <v>297</v>
+      </c>
+      <c r="B273" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2">
+      <c r="A274" t="s">
+        <v>298</v>
+      </c>
+      <c r="B274" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2">
+      <c r="A275" t="s">
+        <v>299</v>
+      </c>
+      <c r="B275" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2">
+      <c r="A276" t="s">
+        <v>300</v>
+      </c>
+      <c r="B276" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2">
+      <c r="A277" t="s">
+        <v>301</v>
+      </c>
+      <c r="B277" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2">
+      <c r="A278" t="s">
+        <v>302</v>
+      </c>
+      <c r="B278" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2">
+      <c r="A279" t="s">
+        <v>303</v>
+      </c>
+      <c r="B279" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2">
+      <c r="A280" t="s">
+        <v>304</v>
+      </c>
+      <c r="B280" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2">
+      <c r="A281" t="s">
+        <v>305</v>
+      </c>
+      <c r="B281" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2">
+      <c r="A282" t="s">
+        <v>306</v>
+      </c>
+      <c r="B282" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2">
+      <c r="A283" t="s">
+        <v>307</v>
+      </c>
+      <c r="B283" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2">
+      <c r="A284" t="s">
+        <v>308</v>
+      </c>
+      <c r="B284" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2">
+      <c r="A285" t="s">
+        <v>309</v>
+      </c>
+      <c r="B285" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2">
+      <c r="A286" t="s">
+        <v>310</v>
+      </c>
+      <c r="B286" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2">
+      <c r="A287" t="s">
+        <v>311</v>
+      </c>
+      <c r="B287" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2">
+      <c r="A288" t="s">
+        <v>312</v>
+      </c>
+      <c r="B288" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2">
+      <c r="A289" t="s">
+        <v>293</v>
+      </c>
+      <c r="B289" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2">
+      <c r="A290" t="s">
+        <v>313</v>
+      </c>
+      <c r="B290" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2">
+      <c r="A291" t="s">
+        <v>314</v>
+      </c>
+      <c r="B291" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2">
+      <c r="A292" t="s">
+        <v>315</v>
+      </c>
+      <c r="B292" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2">
+      <c r="A293" t="s">
+        <v>316</v>
+      </c>
+      <c r="B293" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2">
+      <c r="A294" t="s">
+        <v>317</v>
+      </c>
+      <c r="B294" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2">
+      <c r="A295" t="s">
+        <v>318</v>
+      </c>
+      <c r="B295" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2">
+      <c r="A296" t="s">
+        <v>319</v>
+      </c>
+      <c r="B296" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2">
+      <c r="A297" t="s">
+        <v>320</v>
+      </c>
+      <c r="B297" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2">
+      <c r="A298" t="s">
+        <v>321</v>
+      </c>
+      <c r="B298" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2">
+      <c r="A299" t="s">
+        <v>322</v>
+      </c>
+      <c r="B299" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2">
+      <c r="A300" t="s">
+        <v>323</v>
+      </c>
+      <c r="B300" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2">
+      <c r="A301" t="s">
+        <v>324</v>
+      </c>
+      <c r="B301" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2">
+      <c r="A302" t="s">
+        <v>325</v>
+      </c>
+      <c r="B302" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2">
+      <c r="A303" t="s">
+        <v>326</v>
+      </c>
+      <c r="B303" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2">
+      <c r="A304" t="s">
+        <v>327</v>
+      </c>
+      <c r="B304" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2">
+      <c r="A305" t="s">
+        <v>328</v>
+      </c>
+      <c r="B305" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2">
+      <c r="A306" t="s">
+        <v>329</v>
+      </c>
+      <c r="B306" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2">
+      <c r="A307" t="s">
+        <v>330</v>
+      </c>
+      <c r="B307" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2">
+      <c r="A308" t="s">
+        <v>331</v>
+      </c>
+      <c r="B308" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2">
+      <c r="A309" t="s">
+        <v>332</v>
+      </c>
+      <c r="B309" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2">
+      <c r="A310" t="s">
+        <v>333</v>
+      </c>
+      <c r="B310" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2">
+      <c r="A311" t="s">
+        <v>334</v>
+      </c>
+      <c r="B311" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2">
+      <c r="A312" t="s">
+        <v>335</v>
+      </c>
+      <c r="B312" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2">
+      <c r="A313" t="s">
+        <v>336</v>
+      </c>
+      <c r="B313" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2">
+      <c r="A314" t="s">
+        <v>333</v>
+      </c>
+      <c r="B314" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2">
+      <c r="A315" t="s">
+        <v>337</v>
+      </c>
+      <c r="B315" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2">
+      <c r="A316" t="s">
+        <v>338</v>
+      </c>
+      <c r="B316" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2">
+      <c r="A317" t="s">
+        <v>293</v>
+      </c>
+      <c r="B317" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2">
+      <c r="A318" t="s">
+        <v>339</v>
+      </c>
+      <c r="B318" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2">
+      <c r="A319" t="s">
+        <v>314</v>
+      </c>
+      <c r="B319" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2">
+      <c r="A320" t="s">
+        <v>340</v>
+      </c>
+      <c r="B320" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2">
+      <c r="A321" t="s">
+        <v>341</v>
+      </c>
+      <c r="B321" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2">
+      <c r="A322" t="s">
+        <v>342</v>
+      </c>
+      <c r="B322" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2">
+      <c r="A323" t="s">
+        <v>343</v>
+      </c>
+      <c r="B323" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2">
+      <c r="A324" t="s">
+        <v>344</v>
+      </c>
+      <c r="B324" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2">
+      <c r="A325" t="s">
+        <v>345</v>
+      </c>
+      <c r="B325" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2">
+      <c r="A326" t="s">
+        <v>347</v>
+      </c>
+      <c r="B326" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2">
+      <c r="A327" t="s">
+        <v>322</v>
+      </c>
+      <c r="B327" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2">
+      <c r="A328" t="s">
+        <v>348</v>
+      </c>
+      <c r="B328" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2">
+      <c r="A329" t="s">
+        <v>349</v>
+      </c>
+      <c r="B329" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2">
+      <c r="A330" t="s">
+        <v>351</v>
+      </c>
+      <c r="B330" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2">
+      <c r="A331" t="s">
+        <v>352</v>
+      </c>
+      <c r="B331" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2">
+      <c r="A332" t="s">
+        <v>353</v>
+      </c>
+      <c r="B332" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2">
+      <c r="A333" t="s">
+        <v>354</v>
+      </c>
+      <c r="B333" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2">
+      <c r="A334" t="s">
+        <v>355</v>
+      </c>
+      <c r="B334" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2">
+      <c r="A335" t="s">
+        <v>356</v>
+      </c>
+      <c r="B335" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2">
+      <c r="A336" t="s">
+        <v>357</v>
+      </c>
+      <c r="B336" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2">
+      <c r="A337" t="s">
+        <v>358</v>
+      </c>
+      <c r="B337" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2">
+      <c r="A338" t="s">
+        <v>359</v>
+      </c>
+      <c r="B338" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2">
+      <c r="A339" t="s">
+        <v>360</v>
+      </c>
+      <c r="B339" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2">
+      <c r="A340" t="s">
+        <v>361</v>
+      </c>
+      <c r="B340" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2">
+      <c r="A341" t="s">
+        <v>362</v>
+      </c>
+      <c r="B341" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2">
+      <c r="A342" t="s">
+        <v>363</v>
+      </c>
+      <c r="B342" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2">
+      <c r="A343" t="s">
+        <v>364</v>
+      </c>
+      <c r="B343" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2">
+      <c r="A344" t="s">
+        <v>365</v>
+      </c>
+      <c r="B344" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2">
+      <c r="A345" t="s">
+        <v>366</v>
+      </c>
+      <c r="B345" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2">
+      <c r="A346" t="s">
+        <v>367</v>
+      </c>
+      <c r="B346" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2">
+      <c r="A347" t="s">
+        <v>368</v>
+      </c>
+      <c r="B347" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2">
+      <c r="A348" t="s">
+        <v>369</v>
+      </c>
+      <c r="B348" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2">
+      <c r="A349" t="s">
+        <v>370</v>
+      </c>
+      <c r="B349" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2">
+      <c r="A350" t="s">
+        <v>371</v>
+      </c>
+      <c r="B350" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2">
+      <c r="A351" t="s">
+        <v>373</v>
+      </c>
+      <c r="B351" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2">
+      <c r="A352" t="s">
+        <v>374</v>
+      </c>
+      <c r="B352" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2">
+      <c r="A353" t="s">
+        <v>375</v>
+      </c>
+      <c r="B353" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2">
+      <c r="A354" t="s">
+        <v>376</v>
+      </c>
+      <c r="B354" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2">
+      <c r="A355" t="s">
+        <v>377</v>
+      </c>
+      <c r="B355" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2">
+      <c r="A356" t="s">
+        <v>378</v>
+      </c>
+      <c r="B356" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2">
+      <c r="A357" t="s">
+        <v>379</v>
+      </c>
+      <c r="B357" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2">
+      <c r="A358" t="s">
+        <v>380</v>
+      </c>
+      <c r="B358" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2">
+      <c r="A359" t="s">
+        <v>381</v>
+      </c>
+      <c r="B359" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2">
+      <c r="A360" t="s">
+        <v>382</v>
+      </c>
+      <c r="B360" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2">
+      <c r="A361" t="s">
+        <v>383</v>
+      </c>
+      <c r="B361" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2">
+      <c r="A362" t="s">
+        <v>384</v>
+      </c>
+      <c r="B362" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2">
+      <c r="A363" t="s">
+        <v>385</v>
+      </c>
+      <c r="B363" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2">
+      <c r="A364" t="s">
+        <v>386</v>
+      </c>
+      <c r="B364" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2">
+      <c r="A365" t="s">
+        <v>387</v>
+      </c>
+      <c r="B365" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2">
+      <c r="A366" t="s">
+        <v>389</v>
+      </c>
+      <c r="B366" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2">
+      <c r="A367" t="s">
+        <v>391</v>
+      </c>
+      <c r="B367" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2">
+      <c r="A368" t="s">
+        <v>392</v>
+      </c>
+      <c r="B368" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2">
+      <c r="A369" t="s">
+        <v>393</v>
+      </c>
+      <c r="B369" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2">
+      <c r="A370" t="s">
+        <v>394</v>
+      </c>
+      <c r="B370" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2">
+      <c r="A371" t="s">
+        <v>395</v>
+      </c>
+      <c r="B371" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2">
+      <c r="A372" t="s">
+        <v>396</v>
+      </c>
+      <c r="B372" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2">
+      <c r="A373" t="s">
+        <v>397</v>
+      </c>
+      <c r="B373" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2">
+      <c r="A374" t="s">
+        <v>398</v>
+      </c>
+      <c r="B374" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2">
+      <c r="A375" t="s">
+        <v>399</v>
+      </c>
+      <c r="B375" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2">
+      <c r="A376" t="s">
+        <v>400</v>
+      </c>
+      <c r="B376" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2">
+      <c r="A377" t="s">
+        <v>401</v>
+      </c>
+      <c r="B377" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2">
+      <c r="A378" t="s">
+        <v>402</v>
+      </c>
+      <c r="B378" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2">
+      <c r="A379" t="s">
+        <v>403</v>
+      </c>
+      <c r="B379" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2">
+      <c r="A380" t="s">
+        <v>404</v>
+      </c>
+      <c r="B380" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2">
+      <c r="A381" t="s">
+        <v>405</v>
+      </c>
+      <c r="B381" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2">
+      <c r="A382" t="s">
+        <v>406</v>
+      </c>
+      <c r="B382" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2">
+      <c r="A383" t="s">
+        <v>407</v>
+      </c>
+      <c r="B383" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2">
+      <c r="A384" t="s">
+        <v>408</v>
+      </c>
+      <c r="B384" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2">
+      <c r="A385" t="s">
+        <v>409</v>
+      </c>
+      <c r="B385" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2">
+      <c r="A386" t="s">
+        <v>410</v>
+      </c>
+      <c r="B386" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2">
+      <c r="A387" t="s">
+        <v>411</v>
+      </c>
+      <c r="B387" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2">
+      <c r="A388" t="s">
+        <v>412</v>
+      </c>
+      <c r="B388" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2">
+      <c r="A389" t="s">
+        <v>413</v>
+      </c>
+      <c r="B389" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2">
+      <c r="A390" t="s">
+        <v>415</v>
+      </c>
+      <c r="B390" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2">
+      <c r="A391" t="s">
+        <v>416</v>
+      </c>
+      <c r="B391" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2">
+      <c r="A392" t="s">
+        <v>417</v>
+      </c>
+      <c r="B392" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2">
+      <c r="A393" t="s">
+        <v>418</v>
+      </c>
+      <c r="B393" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2">
+      <c r="A394" t="s">
+        <v>419</v>
+      </c>
+      <c r="B394" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2">
+      <c r="A395" t="s">
+        <v>420</v>
+      </c>
+      <c r="B395" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2">
+      <c r="A396" t="s">
+        <v>421</v>
+      </c>
+      <c r="B396" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2">
+      <c r="A397" t="s">
+        <v>422</v>
+      </c>
+      <c r="B397" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2">
+      <c r="A398" t="s">
+        <v>423</v>
+      </c>
+      <c r="B398" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2">
+      <c r="A399" t="s">
+        <v>424</v>
+      </c>
+      <c r="B399" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2">
+      <c r="A400" t="s">
+        <v>425</v>
+      </c>
+      <c r="B400" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2">
+      <c r="A401" t="s">
+        <v>426</v>
+      </c>
+      <c r="B401" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2">
+      <c r="A402" t="s">
+        <v>427</v>
+      </c>
+      <c r="B402" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2">
+      <c r="A403" t="s">
+        <v>428</v>
+      </c>
+      <c r="B403" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2">
+      <c r="A404" t="s">
+        <v>429</v>
+      </c>
+      <c r="B404" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2">
+      <c r="A405" t="s">
+        <v>430</v>
+      </c>
+      <c r="B405" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2">
+      <c r="A406" t="s">
+        <v>431</v>
+      </c>
+      <c r="B406" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2">
+      <c r="A407" t="s">
+        <v>432</v>
+      </c>
+      <c r="B407" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2">
+      <c r="A408" t="s">
+        <v>433</v>
+      </c>
+      <c r="B408" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2">
+      <c r="A409" t="s">
+        <v>434</v>
+      </c>
+      <c r="B409" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2">
+      <c r="A410" t="s">
+        <v>435</v>
+      </c>
+      <c r="B410" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2">
+      <c r="A411" t="s">
+        <v>436</v>
+      </c>
+      <c r="B411" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2">
+      <c r="A412" t="s">
+        <v>437</v>
+      </c>
+      <c r="B412" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2">
+      <c r="A413" t="s">
+        <v>438</v>
+      </c>
+      <c r="B413" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2">
+      <c r="A414" t="s">
+        <v>439</v>
+      </c>
+      <c r="B414" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2">
+      <c r="A415" t="s">
+        <v>440</v>
+      </c>
+      <c r="B415" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2">
+      <c r="A416" t="s">
+        <v>441</v>
+      </c>
+      <c r="B416" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2">
+      <c r="A417" t="s">
+        <v>443</v>
+      </c>
+      <c r="B417" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2">
+      <c r="A418" t="s">
+        <v>444</v>
+      </c>
+      <c r="B418" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2">
+      <c r="A419" t="s">
+        <v>445</v>
+      </c>
+      <c r="B419" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2">
+      <c r="A420" t="s">
+        <v>446</v>
+      </c>
+      <c r="B420" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2">
+      <c r="A421" t="s">
+        <v>447</v>
+      </c>
+      <c r="B421" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2">
+      <c r="A422" t="s">
+        <v>448</v>
+      </c>
+      <c r="B422" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2">
+      <c r="A423" t="s">
+        <v>449</v>
+      </c>
+      <c r="B423" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2">
+      <c r="A424" t="s">
+        <v>450</v>
+      </c>
+      <c r="B424" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2">
+      <c r="A425" t="s">
+        <v>451</v>
+      </c>
+      <c r="B425" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2">
+      <c r="A426" t="s">
+        <v>452</v>
+      </c>
+      <c r="B426" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2">
+      <c r="A427" t="s">
+        <v>453</v>
+      </c>
+      <c r="B427" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2">
+      <c r="A428" t="s">
+        <v>455</v>
+      </c>
+      <c r="B428" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>